<commit_message>
null answer send from desktop app bug FIXED
nullable answer send from desktop app bug fixed. User can submit without choosing all answer
</commit_message>
<xml_diff>
--- a/static/sample/import_question_sample.xlsx
+++ b/static/sample/import_question_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Online-Examination-System\static\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\KIT Online Examination System\Web App -Online Examination System\static\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13838F8-392F-4EFE-95B7-DC74FDE01E4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FA1494-A5BA-4148-A3A0-ADA2AFCDF48E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1196,8 +1196,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,7 +2338,7 @@
         <v>104</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>